<commit_message>
Guardar automáticamente el commit P3 dom ago 16 22:17:05 -05 2020
</commit_message>
<xml_diff>
--- a/mp3/cortar extraer partes de un mp3 con FFmpeg/Tabla para calcular el tiempo a cortar en minutos a HH-MM-SS.xlsx
+++ b/mp3/cortar extraer partes de un mp3 con FFmpeg/Tabla para calcular el tiempo a cortar en minutos a HH-MM-SS.xlsx
@@ -5,7 +5,7 @@
   <workbookPr/>
   <workbookProtection/>
   <bookViews>
-    <workbookView windowWidth="19584" windowHeight="7588" tabRatio="500" activeTab="1"/>
+    <workbookView windowWidth="19584" windowHeight="7588" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="30 min" sheetId="1" r:id="rId1"/>
@@ -479,10 +479,10 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
-    <numFmt numFmtId="43" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
-    <numFmt numFmtId="42" formatCode="_-&quot;£&quot;* #,##0_-;\-&quot;£&quot;* #,##0_-;_-&quot;£&quot;* &quot;-&quot;_-;_-@_-"/>
     <numFmt numFmtId="44" formatCode="_-&quot;£&quot;* #,##0.00_-;\-&quot;£&quot;* #,##0.00_-;_-&quot;£&quot;* &quot;-&quot;??_-;_-@_-"/>
     <numFmt numFmtId="41" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
+    <numFmt numFmtId="42" formatCode="_-&quot;£&quot;* #,##0_-;\-&quot;£&quot;* #,##0_-;_-&quot;£&quot;* &quot;-&quot;_-;_-@_-"/>
+    <numFmt numFmtId="43" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
   </numFmts>
   <fonts count="34">
     <font>
@@ -517,25 +517,9 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="0"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
+      <sz val="10"/>
+      <name val="FreeSans"/>
+      <charset val="134"/>
     </font>
     <font>
       <sz val="10"/>
@@ -544,68 +528,8 @@
       <charset val="134"/>
     </font>
     <font>
-      <sz val="10"/>
-      <color rgb="FF000000"/>
-      <name val="FreeSans"/>
-      <charset val="134"/>
-    </font>
-    <font>
-      <b/>
       <sz val="11"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="13"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -619,16 +543,16 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
       <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
+      <color rgb="FF3F3F76"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
       <sz val="11"/>
-      <color rgb="FF3F3F76"/>
+      <color rgb="FF3F3F3F"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -650,18 +574,75 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <u/>
       <sz val="11"/>
-      <color rgb="FF800080"/>
+      <color theme="0"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
+      <sz val="13"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <sz val="10"/>
-      <color rgb="FF006600"/>
+      <color rgb="FF000000"/>
       <name val="FreeSans"/>
       <charset val="134"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF808080"/>
+      <name val="FreeSans"/>
+      <charset val="134"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
@@ -671,14 +652,38 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <sz val="10"/>
       <color rgb="FFFFFFFF"/>
       <name val="FreeSans"/>
       <charset val="134"/>
     </font>
     <font>
+      <u/>
       <sz val="11"/>
-      <color rgb="FF9C6500"/>
+      <color rgb="FF800080"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -691,18 +696,13 @@
     </font>
     <font>
       <sz val="10"/>
+      <color rgb="FF333333"/>
       <name val="FreeSans"/>
       <charset val="134"/>
     </font>
     <font>
       <sz val="10"/>
-      <color rgb="FF808080"/>
-      <name val="FreeSans"/>
-      <charset val="134"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <color rgb="FF333333"/>
+      <color rgb="FF006600"/>
       <name val="FreeSans"/>
       <charset val="134"/>
     </font>
@@ -727,13 +727,169 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
+        <fgColor theme="5" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFDDDDDD"/>
+        <bgColor rgb="FFFFCCCC"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFCC0000"/>
+        <bgColor rgb="FF800000"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -745,86 +901,14 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor rgb="FF808080"/>
+        <bgColor rgb="FF969696"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor rgb="FFFFCCCC"/>
         <bgColor rgb="FFDDDDDD"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFDDDDDD"/>
-        <bgColor rgb="FFFFCCCC"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
@@ -835,13 +919,19 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor rgb="FFFFFFFF"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
+        <fgColor theme="9" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -853,103 +943,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFCC0000"/>
-        <bgColor rgb="FF800000"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FF808080"/>
-        <bgColor rgb="FF969696"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor rgb="FFFFFFFF"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor rgb="FF000000"/>
         <bgColor rgb="FF003300"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
+        <fgColor theme="9" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -965,9 +965,11 @@
     <border>
       <left/>
       <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
+        <color theme="4"/>
       </bottom>
       <diagonal/>
     </border>
@@ -983,24 +985,6 @@
       </top>
       <bottom style="thin">
         <color rgb="FF7F7F7F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4"/>
       </bottom>
       <diagonal/>
     </border>
@@ -1022,11 +1006,18 @@
     <border>
       <left/>
       <right/>
-      <top style="thin">
+      <top/>
+      <bottom style="medium">
         <color theme="4"/>
-      </top>
-      <bottom style="double">
-        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
       </bottom>
       <diagonal/>
     </border>
@@ -1042,6 +1033,15 @@
       </top>
       <bottom style="double">
         <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
       </bottom>
       <diagonal/>
     </border>
@@ -1078,154 +1078,154 @@
   </borders>
   <cellStyleXfs count="65">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="31" fillId="35" borderId="9" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="24" fillId="22" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="28" fillId="35" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="26" fillId="36" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="26" fillId="28" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="7" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="7" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="26" fillId="27" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="25" fillId="31" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="25" fillId="38" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="29" fillId="34" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="31" fillId="37" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="30" fillId="34" borderId="9" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="13" fillId="39" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="7" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="38" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="37" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="39" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="13" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="26" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="13" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="36" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="27" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="16" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="7" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="11" fillId="6" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="7" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="22" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="9" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="7" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="27" fillId="4" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="13" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="5" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="17" fillId="6" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="32" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="10" fillId="4" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="43" fontId="0" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="20" fillId="17" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="26" borderId="8" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="3" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="23" borderId="8" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="41" fontId="0" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="28" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -1264,15 +1264,15 @@
   </cellXfs>
   <cellStyles count="65">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Heading" xfId="1"/>
-    <cellStyle name="Note" xfId="2"/>
-    <cellStyle name="Footnote" xfId="3"/>
-    <cellStyle name="Status" xfId="4"/>
+    <cellStyle name="Accent 2" xfId="1"/>
+    <cellStyle name="Accent 1" xfId="2"/>
+    <cellStyle name="Accent" xfId="3"/>
+    <cellStyle name="Neutral" xfId="4"/>
     <cellStyle name="Good" xfId="5"/>
-    <cellStyle name="Neutral" xfId="6"/>
-    <cellStyle name="Accent" xfId="7"/>
-    <cellStyle name="Accent 1" xfId="8"/>
-    <cellStyle name="Accent 2" xfId="9"/>
+    <cellStyle name="Status" xfId="6"/>
+    <cellStyle name="Footnote" xfId="7"/>
+    <cellStyle name="Note" xfId="8"/>
+    <cellStyle name="Heading" xfId="9"/>
     <cellStyle name="60% - Énfasis6" xfId="10" builtinId="52"/>
     <cellStyle name="40% - Énfasis6" xfId="11" builtinId="51"/>
     <cellStyle name="20% - Énfasis5" xfId="12" builtinId="46"/>
@@ -1323,8 +1323,8 @@
     <cellStyle name="Total" xfId="57" builtinId="25"/>
     <cellStyle name="Énfasis3" xfId="58" builtinId="37"/>
     <cellStyle name="40% - Énfasis2" xfId="59" builtinId="35"/>
-    <cellStyle name="Text" xfId="60"/>
-    <cellStyle name="Warning" xfId="61"/>
+    <cellStyle name="Warning" xfId="60"/>
+    <cellStyle name="Text" xfId="61"/>
     <cellStyle name="20% - Énfasis3" xfId="62" builtinId="38"/>
     <cellStyle name="Coma [0]" xfId="63" builtinId="6"/>
     <cellStyle name="Texto de advertencia" xfId="64" builtinId="11"/>
@@ -1666,8 +1666,8 @@
   <sheetPr/>
   <dimension ref="A1:G35"/>
   <sheetViews>
-    <sheetView zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="F9" sqref="F9"/>
+    <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="12.95" outlineLevelCol="6"/>
@@ -2349,8 +2349,8 @@
   <sheetPr/>
   <dimension ref="A1:G35"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" topLeftCell="A11" workbookViewId="0">
-      <selection activeCell="G33" sqref="G33"/>
+    <sheetView zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="12.95" outlineLevelCol="6"/>
@@ -2367,7 +2367,6 @@
       <c r="B1" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="1"/>
       <c r="D1" s="5" t="s">
         <v>1</v>
       </c>
@@ -3035,7 +3034,7 @@
   <dimension ref="A1:G35"/>
   <sheetViews>
     <sheetView zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="12.95" outlineLevelCol="6"/>
@@ -3052,7 +3051,6 @@
       <c r="B1" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="1"/>
       <c r="D1" s="5" t="s">
         <v>1</v>
       </c>

</xml_diff>